<commit_message>
Updating code for trade tables.
Having issues with the value for animalProducts
</commit_message>
<xml_diff>
--- a/data/open/OPN_FINAL_ASY_BECClassifications_31-01-20.xlsx
+++ b/data/open/OPN_FINAL_ASY_BECClassifications_31-01-20.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hugopigott/Dropbox/2. Work/Repositories/vnso-RAP-tradeStats-materials/data/open/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D75D648-646B-FF45-9DFA-ABFA63E85123}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F046C39D-F1BD-2049-84F8-D84F7A3771DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15717,7 +15717,7 @@
     <t>890710</t>
   </si>
   <si>
-    <t>HS6</t>
+    <t>HS.Code_6</t>
   </si>
 </sst>
 </file>
@@ -15761,9 +15761,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -16047,7 +16048,7 @@
   <dimension ref="A1:D5205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16056,7 +16057,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>5230</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>